<commit_message>
fix: update database files and improve init_db script formatting; fix: cadastro regras dados de distribuicao por uc por eixo no banco tf_cadastro_regras_negocios;
</commit_message>
<xml_diff>
--- a/dados/base_iniciativas_resumos_sei.xlsx
+++ b/dados/base_iniciativas_resumos_sei.xlsx
@@ -1,39 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28429"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dmagi\Downloads\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F454A2D-2A4C-4B34-A743-DB268A518C13}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-10875" windowWidth="38640" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
+    <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
   </sheets>
-  <calcPr calcId="191029"/>
-  <extLst>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
   <si>
     <t>Diretoria</t>
   </si>
@@ -47,6 +28,9 @@
     <t>Demandante</t>
   </si>
   <si>
+    <t>id_resumo</t>
+  </si>
+  <si>
     <t>Iniciativa</t>
   </si>
   <si>
@@ -72,6 +56,9 @@
   </si>
   <si>
     <t>Coordenação de Fiscalização - COFIS</t>
+  </si>
+  <si>
+    <t>DIMAN</t>
   </si>
   <si>
     <t>Proposta de captação de recursos da compensação ambiental para o fortalecimento da estratégia e 
@@ -447,6 +434,9 @@
     <t>Coordenação Geral de Gestão Socioambiental - CGSAM</t>
   </si>
   <si>
+    <t>DISAT</t>
+  </si>
+  <si>
     <t>Fortalecendo a participação social nas Ações de Gestão Socioambiental nas UCs federais.</t>
   </si>
   <si>
@@ -620,6 +610,9 @@
   </si>
   <si>
     <t>Coordenação de Monitoramento da Biodiversidade - COMOB</t>
+  </si>
+  <si>
+    <t>DIBIO</t>
   </si>
   <si>
     <t xml:space="preserve">Proposta de captação de recursos da compensação ambiental 
@@ -1220,29 +1213,73 @@
 %A7%C3%A3o/Guia-de-Restauracao-Ecologica_digital.pdf</t>
   </si>
   <si>
-    <t>id_resumo</t>
-  </si>
-  <si>
-    <t>DIMAN</t>
-  </si>
-  <si>
-    <t>DISAT</t>
-  </si>
-  <si>
-    <t>DIBIO</t>
+    <t>Divisão de Gestão Territorial Integrada - DGTI/CGCAP</t>
+  </si>
+  <si>
+    <t>Reconhecimento e Implementação de Mosaicos de Áreas Protegidas</t>
+  </si>
+  <si>
+    <t>Diante da importância de UCs bem geridas para a conservação, a Convenção para a Diversidade Biológica incluiu entre as Metas de Aichi, não só a necessidade de aumentar o número de áreas sob proteção, mas que estas áreas também sejam “administradas de maneira eficaz e equitativa” (CDB, 2010). O estabelecimento dessas áreas protegidas é considerado a melhor estratégia para conservar in situ a biodiversidade em longo prazo (Primack e Rodrigues, 2002) Uma das estratégias associadas a implementação das unidades de conservação é a instituição de mosaicos de UCs que interliguem áreas protegidas próximas ou justa postas, segundo o art. 26 a lei no 9.985, de 18 de julho de 2000.</t>
+  </si>
+  <si>
+    <t>A conservação da biodiversidade e a proteção dos ecossistemas naturais são imperativos cada vez mais prementes em um mundo em rápida transformação. Nesse contexto, as unidades de conservação (UCs) e demais áreas especialmente protegidas, desempenham um papel fundamental na preservação dos recursos naturais e na promoção do desenvolvimento sustentável. No entanto, a eficácia desses espaços protegidos muitas vezes é limitada pela fragmentação do habitat e pela falta de conectividade entre diferentes UCs. Esta proposta elenca os mosaicos como uma das estratégias institucionais para melhoria da gestão territorial integrada nos territórios em que as UCs estão inseridas. Assim, busca dirimir lacunas para reconhecimento de novos mosaicos, bem como auxílio na implementação dos mosaicos já existentes. Para gestão dos mosaicos é imperioso o estabelecimento do seu conselho, que geralmente ocorre no ato de reconhecimento, e seu funcionamento depende de realizações de reuniões e equipamentos adequados para tal.</t>
+  </si>
+  <si>
+    <t>Estabelecimento de novos mosaicos de áreas protegidas e auxílio na implementação dos planos de gestão territorial</t>
+  </si>
+  <si>
+    <t>ESEC Da Guanabara, ESEC de Guaraqueçaba, ESEC de Tamoios, ESEC de Tupiniquins, PARNA da Serra da Bocaina, PARNA da Serra dos Órgãos, PARNA de Saint-Hilaire/Lange, PARNA do Monte Pascoal, REBIO de Comboios, REBIO de Sooretama, REBIO do Tinguá, REBIO União, RESEX Corumbau e RESEX Mandira.</t>
+  </si>
+  <si>
+    <t>Considerando os referenciais teóricos listados acima, bem como os destaques elencados da estratégia proposta neste resumo executivo.
+Para alcance de tamanho desafio as seguintes atividades podem ser apoiadas:
+a) Para apoiar criação de mosaicos:
+▪ Vistorias 
+▪ Reuniões com atores externos e internos
+▪ Aquisição de equipamentos
+▪ Análises geográfcias
+▪ Elaboração de memoriais descritivos
+▪ Definição do escopo do mosaicos
+▪ Elaboração de Notas técnicas para reconhecimento de mosaicos
+▪ Contratação de consultor qualificado
+▪ Aluguel de veículos
+▪ Realização de consultas públicas e demais eventos;
+b) Para apoiar a implementação dos Mosaicos:
+➢ Quanto ao apoio as reuniões do conselho do mosaico:
+▪ Apoia para realização da reunião do conselho
+▪ Realização de eventos
+▪ Aquisição e equipamento
+▪ Contratação de secretária executiva do conselho
+➢ Quanto ao apoio a implementação dos planejamentos territoriais:
+▪ Atividades diversas relacionadas nos planejamentos territoriais que 
+estejam afetas as unidades de conservação, 
+Em relação aos insumos que serão utilizados para cada uma das atividades listadas, podem 
+ser compartilhados e através de contrapartidas se complementarem as necessidades das 
+atividades conforme a disponibilidade da execução via compensação ambiental bem como 
+adas estratégia institucionais definidas para determinado mosaico.
+Considerando que este resumo abrange duas frentes de trabalho quais sejam: 1) 
+Estabelecimento de novos mosaicos (SEI )e 2) Implementação dos mosaicos existentes, (SEI 
+) apresentamos duas planilhas de Planilha_Indicacao_de_Recursos_Iniciativas_estrategicas, sendo uma para cada frente de trabalho destacada</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
+  <numFmts count="0"/>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -1253,7 +1290,14 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
     <border>
       <left/>
       <right/>
@@ -1265,20 +1309,32 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+  <cellXfs count="6">
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+      <alignment horizontal="general"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle xfId="0" builtinId="0" name="Normal"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1289,10 +1345,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -1330,71 +1386,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Times New Roman"/>
-        <a:font script="Hebr" typeface="Times New Roman"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="MoolBoran"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Times New Roman"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Times New Roman" script="Arab"/>
+        <a:font typeface="Times New Roman" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="MoolBoran" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Times New Roman" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
-        <a:font script="Hang" typeface="맑은 고딕"/>
-        <a:font script="Hans" typeface="宋体"/>
-        <a:font script="Hant" typeface="新細明體"/>
-        <a:font script="Arab" typeface="Arial"/>
-        <a:font script="Hebr" typeface="Arial"/>
-        <a:font script="Thai" typeface="Tahoma"/>
-        <a:font script="Ethi" typeface="Nyala"/>
-        <a:font script="Beng" typeface="Vrinda"/>
-        <a:font script="Gujr" typeface="Shruti"/>
-        <a:font script="Khmr" typeface="DaunPenh"/>
-        <a:font script="Knda" typeface="Tunga"/>
-        <a:font script="Guru" typeface="Raavi"/>
-        <a:font script="Cans" typeface="Euphemia"/>
-        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
-        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
-        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
-        <a:font script="Thaa" typeface="MV Boli"/>
-        <a:font script="Deva" typeface="Mangal"/>
-        <a:font script="Telu" typeface="Gautami"/>
-        <a:font script="Taml" typeface="Latha"/>
-        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
-        <a:font script="Orya" typeface="Kalinga"/>
-        <a:font script="Mlym" typeface="Kartika"/>
-        <a:font script="Laoo" typeface="DokChampa"/>
-        <a:font script="Sinh" typeface="Iskoola Pota"/>
-        <a:font script="Mong" typeface="Mongolian Baiti"/>
-        <a:font script="Viet" typeface="Arial"/>
-        <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
+        <a:font typeface="맑은 고딕" script="Hang"/>
+        <a:font typeface="宋体" script="Hans"/>
+        <a:font typeface="新細明體" script="Hant"/>
+        <a:font typeface="Arial" script="Arab"/>
+        <a:font typeface="Arial" script="Hebr"/>
+        <a:font typeface="Tahoma" script="Thai"/>
+        <a:font typeface="Nyala" script="Ethi"/>
+        <a:font typeface="Vrinda" script="Beng"/>
+        <a:font typeface="Shruti" script="Gujr"/>
+        <a:font typeface="DaunPenh" script="Khmr"/>
+        <a:font typeface="Tunga" script="Knda"/>
+        <a:font typeface="Raavi" script="Guru"/>
+        <a:font typeface="Euphemia" script="Cans"/>
+        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
+        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
+        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
+        <a:font typeface="MV Boli" script="Thaa"/>
+        <a:font typeface="Mangal" script="Deva"/>
+        <a:font typeface="Gautami" script="Telu"/>
+        <a:font typeface="Latha" script="Taml"/>
+        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
+        <a:font typeface="Kalinga" script="Orya"/>
+        <a:font typeface="Kartika" script="Mlym"/>
+        <a:font typeface="DokChampa" script="Laoo"/>
+        <a:font typeface="Iskoola Pota" script="Sinh"/>
+        <a:font typeface="Mongolian Baiti" script="Mong"/>
+        <a:font typeface="Arial" script="Viet"/>
+        <a:font typeface="Microsoft Uighur" script="Uigh"/>
+        <a:font typeface="Sylfaen" script="Geor"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1422,7 +1478,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1445,11 +1501,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin ang="16200000" scaled="1"/>
+          <a:lin scaled="1" ang="16200000"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1458,13 +1514,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1474,7 +1530,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1483,7 +1539,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1492,7 +1548,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1500,10 +1556,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot lat="0" lon="0" rev="0"/>
+              <a:rot rev="0" lon="0" lat="0"/>
             </a:camera>
-            <a:lightRig rig="threePt" dir="t">
-              <a:rot lat="0" lon="0" rev="1200000"/>
+            <a:lightRig dir="t" rig="threePt">
+              <a:rot rev="1200000" lon="0" lat="0"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1568,426 +1624,562 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K12"/>
+  <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
-    </sheetView>
+    <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="91" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="140.5703125" customWidth="1"/>
-    <col min="7" max="11" width="13.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" style="4" width="91.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="4" width="94.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="4" width="75.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="4" width="140.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="528.75">
+      <c r="A2" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" s="3">
+        <v>10</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="1179">
+      <c r="A3" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3">
+        <v>3</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="261">
+      <c r="A4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E4" s="3">
+        <v>6</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="312">
+      <c r="A5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="E5" s="3">
+        <v>1</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="210">
+      <c r="A6" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6" s="1"/>
+      <c r="D6" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E6" s="3">
+        <v>13</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="567">
+      <c r="A7" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C7" s="1"/>
+      <c r="D7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="3">
+        <v>8</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="528.75">
+      <c r="A8" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E8" s="3">
+        <v>7</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="108">
+      <c r="A9" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="E9" s="3">
+        <v>11</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="H9" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="1319.25">
+      <c r="A10" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B10" s="1"/>
+      <c r="C10" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E10" s="3">
+        <v>2</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H10" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="528.75">
+      <c r="A11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C11" s="1"/>
+      <c r="D11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E11" s="3">
+        <v>5</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="426.75">
+      <c r="A12" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C12" s="1"/>
+      <c r="D12" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="3">
+        <v>4</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="H12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F1" t="s">
-        <v>4</v>
-      </c>
-      <c r="G1" t="s">
-        <v>5</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
-      </c>
-      <c r="I1" t="s">
-        <v>7</v>
-      </c>
-      <c r="J1" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" t="s">
-        <v>9</v>
+      <c r="I12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>97</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" t="s">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="375.75">
+      <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E2">
-        <v>10</v>
-      </c>
-      <c r="F2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" t="s">
+      <c r="B13" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="H2" t="s">
+      <c r="E13" s="2">
         <v>15</v>
       </c>
-      <c r="I2" t="s">
-        <v>16</v>
-      </c>
-      <c r="J2" t="s">
-        <v>17</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
+      <c r="F13" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>104</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" t="s">
-        <v>95</v>
-      </c>
-      <c r="E3">
-        <v>3</v>
-      </c>
-      <c r="F3" t="s">
-        <v>20</v>
-      </c>
-      <c r="G3" t="s">
-        <v>21</v>
-      </c>
-      <c r="H3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J3" t="s">
-        <v>24</v>
-      </c>
-      <c r="K3" t="s">
-        <v>25</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
+      <c r="E14" s="2"/>
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>10</v>
-      </c>
-      <c r="B4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" t="s">
-        <v>27</v>
-      </c>
-      <c r="D4" t="s">
-        <v>95</v>
-      </c>
-      <c r="E4">
-        <v>6</v>
-      </c>
-      <c r="F4" t="s">
-        <v>28</v>
-      </c>
-      <c r="G4" t="s">
-        <v>29</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>31</v>
-      </c>
-      <c r="J4" t="s">
-        <v>32</v>
-      </c>
-      <c r="K4" t="s">
-        <v>33</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+      <c r="A15" s="1"/>
+      <c r="B15" s="1"/>
+      <c r="C15" s="1"/>
+      <c r="D15" s="1"/>
+      <c r="E15" s="2"/>
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+      <c r="I15" s="1"/>
+      <c r="J15" s="1"/>
+      <c r="K15" s="1"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B5" t="s">
-        <v>34</v>
-      </c>
-      <c r="C5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D5" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5" t="s">
-        <v>36</v>
-      </c>
-      <c r="G5" t="s">
-        <v>37</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-      <c r="I5" t="s">
-        <v>39</v>
-      </c>
-      <c r="J5" t="s">
-        <v>40</v>
-      </c>
-      <c r="K5" t="s">
-        <v>41</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+      <c r="A16" s="1"/>
+      <c r="B16" s="1"/>
+      <c r="C16" s="1"/>
+      <c r="D16" s="1"/>
+      <c r="E16" s="2"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-      <c r="D6" t="s">
-        <v>96</v>
-      </c>
-      <c r="E6">
-        <v>13</v>
-      </c>
-      <c r="F6" t="s">
-        <v>44</v>
-      </c>
-      <c r="G6" t="s">
-        <v>45</v>
-      </c>
-      <c r="H6" t="s">
-        <v>46</v>
-      </c>
-      <c r="I6" t="s">
-        <v>47</v>
-      </c>
-      <c r="J6" t="s">
-        <v>48</v>
-      </c>
-      <c r="K6" t="s">
-        <v>49</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+      <c r="A17" s="1"/>
+      <c r="B17" s="1"/>
+      <c r="C17" s="1"/>
+      <c r="D17" s="1"/>
+      <c r="E17" s="2"/>
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" t="s">
-        <v>50</v>
-      </c>
-      <c r="D7" t="s">
-        <v>96</v>
-      </c>
-      <c r="E7">
-        <v>8</v>
-      </c>
-      <c r="F7" t="s">
-        <v>51</v>
-      </c>
-      <c r="G7" t="s">
-        <v>52</v>
-      </c>
-      <c r="H7" t="s">
-        <v>53</v>
-      </c>
-      <c r="I7" t="s">
-        <v>54</v>
-      </c>
-      <c r="J7" t="s">
-        <v>55</v>
-      </c>
-      <c r="K7" t="s">
-        <v>56</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+      <c r="A18" s="1"/>
+      <c r="B18" s="1"/>
+      <c r="C18" s="1"/>
+      <c r="D18" s="1"/>
+      <c r="E18" s="2"/>
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+      <c r="I18" s="1"/>
+      <c r="J18" s="1"/>
+      <c r="K18" s="1"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>57</v>
-      </c>
-      <c r="B8" t="s">
-        <v>58</v>
-      </c>
-      <c r="C8" t="s">
-        <v>59</v>
-      </c>
-      <c r="D8" t="s">
-        <v>97</v>
-      </c>
-      <c r="E8">
-        <v>7</v>
-      </c>
-      <c r="F8" t="s">
-        <v>60</v>
-      </c>
-      <c r="G8" t="s">
-        <v>61</v>
-      </c>
-      <c r="H8" t="s">
-        <v>62</v>
-      </c>
-      <c r="I8" t="s">
-        <v>63</v>
-      </c>
-      <c r="J8" t="s">
-        <v>64</v>
-      </c>
-      <c r="K8" t="s">
-        <v>65</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+      <c r="A19" s="1"/>
+      <c r="B19" s="1"/>
+      <c r="C19" s="1"/>
+      <c r="D19" s="1"/>
+      <c r="E19" s="2"/>
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+      <c r="I19" s="1"/>
+      <c r="J19" s="1"/>
+      <c r="K19" s="1"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>42</v>
-      </c>
-      <c r="B9" t="s">
-        <v>66</v>
-      </c>
-      <c r="D9" t="s">
-        <v>96</v>
-      </c>
-      <c r="E9">
-        <v>11</v>
-      </c>
-      <c r="F9" t="s">
-        <v>67</v>
-      </c>
-      <c r="G9" t="s">
-        <v>68</v>
-      </c>
-      <c r="H9" t="s">
-        <v>69</v>
-      </c>
-      <c r="I9" t="s">
-        <v>70</v>
-      </c>
-      <c r="J9" t="s">
-        <v>71</v>
-      </c>
-      <c r="K9" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>57</v>
-      </c>
-      <c r="C10" t="s">
-        <v>73</v>
-      </c>
-      <c r="D10" t="s">
-        <v>97</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="F10" t="s">
-        <v>74</v>
-      </c>
-      <c r="G10" t="s">
-        <v>75</v>
-      </c>
-      <c r="H10" t="s">
-        <v>76</v>
-      </c>
-      <c r="I10" t="s">
-        <v>77</v>
-      </c>
-      <c r="J10" t="s">
-        <v>78</v>
-      </c>
-      <c r="K10" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" t="s">
-        <v>80</v>
-      </c>
-      <c r="D11" t="s">
-        <v>97</v>
-      </c>
-      <c r="E11">
-        <v>5</v>
-      </c>
-      <c r="F11" t="s">
-        <v>81</v>
-      </c>
-      <c r="G11" t="s">
-        <v>82</v>
-      </c>
-      <c r="H11" t="s">
-        <v>83</v>
-      </c>
-      <c r="I11" t="s">
-        <v>84</v>
-      </c>
-      <c r="J11" t="s">
-        <v>85</v>
-      </c>
-      <c r="K11" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>57</v>
-      </c>
-      <c r="B12" t="s">
-        <v>87</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
-      </c>
-      <c r="E12">
-        <v>4</v>
-      </c>
-      <c r="F12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G12" t="s">
-        <v>89</v>
-      </c>
-      <c r="H12" t="s">
-        <v>90</v>
-      </c>
-      <c r="I12" t="s">
-        <v>91</v>
-      </c>
-      <c r="J12" t="s">
-        <v>92</v>
-      </c>
-      <c r="K12" t="s">
-        <v>93</v>
-      </c>
+    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+      <c r="A20" s="1"/>
+      <c r="B20" s="1"/>
+      <c r="C20" s="1"/>
+      <c r="D20" s="1"/>
+      <c r="E20" s="2"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
fix: consulta tetos + tabelas de dados para download
</commit_message>
<xml_diff>
--- a/dados/base_iniciativas_resumos_sei.xlsx
+++ b/dados/base_iniciativas_resumos_sei.xlsx
@@ -9,12 +9,15 @@
   <sheets>
     <sheet r:id="rId1" sheetId="1" name="Planilha1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0">Planilha1!$A$1:$K$1</definedName>
+  </definedNames>
   <calcPr fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="106">
   <si>
     <t>Diretoria</t>
   </si>
@@ -1219,13 +1222,64 @@
     <t>Reconhecimento e Implementação de Mosaicos de Áreas Protegidas</t>
   </si>
   <si>
-    <t>Diante da importância de UCs bem geridas para a conservação, a Convenção para a Diversidade Biológica incluiu entre as Metas de Aichi, não só a necessidade de aumentar o número de áreas sob proteção, mas que estas áreas também sejam “administradas de maneira eficaz e equitativa” (CDB, 2010). O estabelecimento dessas áreas protegidas é considerado a melhor estratégia para conservar in situ a biodiversidade em longo prazo (Primack e Rodrigues, 2002) Uma das estratégias associadas a implementação das unidades de conservação é a instituição de mosaicos de UCs que interliguem áreas protegidas próximas ou justa postas, segundo o art. 26 a lei no 9.985, de 18 de julho de 2000.</t>
-  </si>
-  <si>
-    <t>A conservação da biodiversidade e a proteção dos ecossistemas naturais são imperativos cada vez mais prementes em um mundo em rápida transformação. Nesse contexto, as unidades de conservação (UCs) e demais áreas especialmente protegidas, desempenham um papel fundamental na preservação dos recursos naturais e na promoção do desenvolvimento sustentável. No entanto, a eficácia desses espaços protegidos muitas vezes é limitada pela fragmentação do habitat e pela falta de conectividade entre diferentes UCs. Esta proposta elenca os mosaicos como uma das estratégias institucionais para melhoria da gestão territorial integrada nos territórios em que as UCs estão inseridas. Assim, busca dirimir lacunas para reconhecimento de novos mosaicos, bem como auxílio na implementação dos mosaicos já existentes. Para gestão dos mosaicos é imperioso o estabelecimento do seu conselho, que geralmente ocorre no ato de reconhecimento, e seu funcionamento depende de realizações de reuniões e equipamentos adequados para tal.</t>
-  </si>
-  <si>
-    <t>Estabelecimento de novos mosaicos de áreas protegidas e auxílio na implementação dos planos de gestão territorial</t>
+    <t>Apesar da importância estratégica das áreas protegidas para a manutenção da 
+sociobiodiversidade, as limitações impostas para a sua implementação têm representado uma 
+constante ameaça para o cumprimento de seus objetivos (Marinelli e Lederman, 2007). e os 
+esforços globais de conservação não têm sido suficientes para contrapor ao aumento das 
+pressões humanas sobre os ecossistemas naturais, e a diversidade biológica continua 
+diminuindo (Butchart et al., 2010).
+Para a manutenção da biodiversidade são necessárias grandes extensões de ecossistemas 
+naturais que sustentam importantes processos ecológicos e evolutivos (BRASIL, 2006). Ela 
+depende, entre outros aspéctos, do fluxo de genes, da troca genética e da movimentação da 
+biota (Ehrlich, P. R.. 1997) e quanto maior forem às áreas protegidas, maiores serão as 
+possibilidades neste sentido
+Diante da importância de UCs bem geridas para a conservação, a Convenção para a 
+Diversidade Biológica incluiu entre as Metas de Aichi, não só a necessidade de aumentar o 
+número de áreas sob proteção, mas que estas áreas também sejam “administradas de maneira 
+eficaz e equitativa” (CDB, 2010). O estabelecimento dessas áreas protegidas é considerado a 
+melhor estratégia para conservar in situ a biodiversidade em longo prazo (Primack e Rodrigues, 
+2002). Uma das estratégias associadas a implementação das unidades de conservação é a instituição 
+de mosaicos de UCs que interliguem áreas protegidas próximas ou justa postas, segundo o art. 
+26 a lei no 9.985, de 18 de julho de 2000. Embora previstos na lei de 2000 sua formalização se inicia apenas em 2005 com a criação do primeiro mosaico de áreas protegidas no Brasil: O Capivara Confusões, criado através da 
+portaria n° 76, de 11/03/2005, uma iniciativa que integrou o Parque Nacional da Serra da 
+Capivara ao Parque Nacional da Serra das Confusões, tendo entre 2006-2009 seu ápice de 
+criação. Na maioria das portarias de criação dos mosaicos, tem-se a instituição do seu conselho, sendo 
+este o principal instrumento de gestão dos mosaicos, assim a avaliação de como estes espaços 
+estão funcionando, observando suas estratégias de funcionamento, métodos de 
+acompanhamento e forma de atendimento das demandas, contribui para a padronização de 
+procedimentos que melhorem a gestão dos mosaicos.
+O decreto Nº 4.340, de 22 de agosto de 2002, que regulamenta artigos da lei 9985/00 já 
+mencionada, destaca que os mosaicos têm, entre outros, “os atributos de propor diretrizes e 
+ações para compatibilizar, integrar e otimizar, as atividades desenvolvidas em cada unidade de 
+conservação e a relação com a população residente na área do mosaico.”
+Assim os mosaicos surgem como uma abordagem inovadora e integradora para superar esses 
+desafios, integrando diferentes áreas protegidas em uma rede coesa e funcional. A 
+implementação de planejamentos territoriais desses mosaicos de UCs federais emerge como 
+uma estratégia essencial para garantir a gestão eficiente e sustentável dessas áreas.
+Como a atuação para a conservação da biodiversidade têm se tornado cada vez mais 
+estratégica e complexa, a necessidade de decisões de gestão adequadas é ainda maior, 
+aumentando o desafio e a responsabilidade dos planejadores (Spoelder et al., 2015).
+Para fortalecer o mosaico como uma ferramenta da gestão integrada de áreas protegidas e 
+para o desenvolvimento sustentável do território é importante que se apliquem instrumentos 
+de planejamento estratégico e operacional, e que sejam definidos e implementados sistemas 
+de avaliação pautados em indicadores específicos para avaliar a efetividade da gestão 
+integrada de mosaicos (Pinheiro, 2010). 
+Para tanto se pretende aplicar parte dos recursos de compensação ambiental das Ucs 
+“mosaicadas” para implementação dos conselhos dos mosaicos, elaboração e execução dos 
+planejamentos territoriais no Brasil.
+Nesse sentido pretende-se aplicar parte dos recursos de compensação ambiental das Ucs 
+“mosaicadas” para implementação dos conselhos dos mosaicos, elaboração e execução dos 
+planejamentos territoriais no Brasil e aferição de indicadores de efetividade de 
+implementação.</t>
+  </si>
+  <si>
+    <t>A conservação da biodiversidade e a proteção dos ecossistemas naturais são imperativos cada vez mais prementes em um mundo em rápida transformação. Nesse contexto, as unidades de conservação (UCs) e demais áreas especialmente protegidas, desempenham um papel fundamental na preservação dos recursos naturais e na promoção do desenvolvimento sustentável. No entanto, a eficácia desses espaços protegidos muitas vezes é limitada pela fragmentação do habitat e pela falta de conectividade entre diferentes UCs.
+Esta proposta elenca os mosaicos como uma das estratégias institucionais para melhoria da gestão territorial integrada nos territórios em que as UCs estão inseridas. 
+Assim, busca dirimir lacunas para reconhecimento de novos mosaicos, bem como auxílio na implementação dos mosaicos já existentes.
+Para gestão dos mosaicos é imperioso o estabelecimento do seu conselho, que geralmente ocorre no ato de reconhecimento, e seu funcionamento depende de realizações de reuniões e equipamentos adequados para tal. Para gestão dos mosaicos é imperioso o estabelecimento do seu conselho, que geralmente ocorre no ato de reconhecimento, e seu funcionamento depende de realizações de reuniões que só podem ser operacionalizadas mediante estrutura física e financeira disponível, como por exemplo equipamentos adequados, profissionais direcionados para as articulações, bem como espaços físicos disponíveis, e recursos que possam custear as despesas advindas das ações. Os planos de desenvolvimentos territoriais devem ser implementados de forma colaborativa e compartilhada entre todos os atores, possuindo ações específicas para os entes, inclusive para o ICMBIO, que deve apoiar e conduzir determinadas ações no território para atingimento dos objetivos destes planos.</t>
+  </si>
+  <si>
+    <t>Estabelecimento de novos mosaicos de áreas protegidas e auxílio na implementação dos planos de gestão territorial.</t>
   </si>
   <si>
     <t>ESEC Da Guanabara, ESEC de Guaraqueçaba, ESEC de Tamoios, ESEC de Tupiniquins, PARNA da Serra da Bocaina, PARNA da Serra dos Órgãos, PARNA de Saint-Hilaire/Lange, PARNA do Monte Pascoal, REBIO de Comboios, REBIO de Sooretama, REBIO do Tinguá, REBIO União, RESEX Corumbau e RESEX Mandira.</t>
@@ -1243,7 +1297,7 @@
 ▪ Elaboração de Notas técnicas para reconhecimento de mosaicos
 ▪ Contratação de consultor qualificado
 ▪ Aluguel de veículos
-▪ Realização de consultas públicas e demais eventos;
+▪ Realização de consultas públicas e demais eventos
 b) Para apoiar a implementação dos Mosaicos:
 ➢ Quanto ao apoio as reuniões do conselho do mosaico:
 ▪ Apoia para realização da reunião do conselho
@@ -1251,15 +1305,13 @@
 ▪ Aquisição e equipamento
 ▪ Contratação de secretária executiva do conselho
 ➢ Quanto ao apoio a implementação dos planejamentos territoriais:
-▪ Atividades diversas relacionadas nos planejamentos territoriais que 
-estejam afetas as unidades de conservação, 
-Em relação aos insumos que serão utilizados para cada uma das atividades listadas, podem 
-ser compartilhados e através de contrapartidas se complementarem as necessidades das 
-atividades conforme a disponibilidade da execução via compensação ambiental bem como 
-adas estratégia institucionais definidas para determinado mosaico.
-Considerando que este resumo abrange duas frentes de trabalho quais sejam: 1) 
-Estabelecimento de novos mosaicos (SEI )e 2) Implementação dos mosaicos existentes, (SEI 
-) apresentamos duas planilhas de Planilha_Indicacao_de_Recursos_Iniciativas_estrategicas, sendo uma para cada frente de trabalho destacada</t>
+▪ Atividades diversas relacionadas nos planejamentos territoriais que estejam afetas as unidades de conservação.
+Em relação aos insumos que serão utilizados para cada uma das atividades listadas, podem ser compartilhados e através de contrapartidas se complementarem as necessidades das atividades conforme a disponibilidade da execução via compensação ambiental bem como adas estratégia institucionais definidas para determinado mosaico.
+Considerando que este resumo abrange duas frentes de trabalho quais sejam: 
+1) Estabelecimento de novos mosaicos e 2) Implementação dos mosaicos existentes, apresentamos duas planilhas de Planilha_Indicacao_de_Recursos_Iniciativas_estrategicas, sendo uma para cada frente de trabalho destacada</t>
+  </si>
+  <si>
+    <t>Planos de Ação Nacional para Conservação de Espécies Ameaçadas de Extinção - PAN</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1319,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1278,6 +1330,12 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -1309,13 +1367,16 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1324,7 +1385,7 @@
       <alignment horizontal="general"/>
     </xf>
     <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1628,23 +1689,23 @@
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:K20"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="1"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="4" width="91.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="4" width="94.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="4" width="75.005" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="4" width="140.57642857142858" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="5" width="91.005" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="94.86214285714286" customWidth="1" bestFit="1"/>
+    <col min="3" max="3" style="5" width="75.005" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="5" max="5" style="6" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="6" max="6" style="5" width="140.57642857142858" customWidth="1" bestFit="1"/>
+    <col min="7" max="7" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="8" max="8" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="9" max="9" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="10" max="10" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
+    <col min="11" max="11" style="5" width="39.57642857142857" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
@@ -2055,7 +2116,7 @@
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="375.75">
+    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="630.75">
       <c r="A13" s="1" t="s">
         <v>11</v>
       </c>
@@ -2068,7 +2129,7 @@
       <c r="D13" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="E13" s="2">
+      <c r="E13" s="4">
         <v>15</v>
       </c>
       <c r="F13" s="1" t="s">
@@ -2090,96 +2151,38 @@
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="1"/>
-      <c r="B14" s="1"/>
+    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="528.75">
+      <c r="A14" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>84</v>
+      </c>
       <c r="C14" s="1"/>
-      <c r="D14" s="1"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="1"/>
-      <c r="G14" s="1"/>
-      <c r="H14" s="1"/>
-      <c r="I14" s="1"/>
-      <c r="J14" s="1"/>
-      <c r="K14" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="1"/>
-      <c r="B15" s="1"/>
-      <c r="C15" s="1"/>
-      <c r="D15" s="1"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="1"/>
-      <c r="B16" s="1"/>
-      <c r="C16" s="1"/>
-      <c r="D16" s="1"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="1"/>
-      <c r="B17" s="1"/>
-      <c r="C17" s="1"/>
-      <c r="D17" s="1"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="1"/>
-      <c r="G17" s="1"/>
-      <c r="H17" s="1"/>
-      <c r="I17" s="1"/>
-      <c r="J17" s="1"/>
-      <c r="K17" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="1"/>
-      <c r="B18" s="1"/>
-      <c r="C18" s="1"/>
-      <c r="D18" s="1"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="1"/>
-      <c r="G18" s="1"/>
-      <c r="H18" s="1"/>
-      <c r="I18" s="1"/>
-      <c r="J18" s="1"/>
-      <c r="K18" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="1"/>
-      <c r="B19" s="1"/>
-      <c r="C19" s="1"/>
-      <c r="D19" s="1"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="1"/>
-      <c r="G19" s="1"/>
-      <c r="H19" s="1"/>
-      <c r="I19" s="1"/>
-      <c r="J19" s="1"/>
-      <c r="K19" s="1"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="1"/>
-      <c r="B20" s="1"/>
-      <c r="C20" s="1"/>
-      <c r="D20" s="1"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="1"/>
-      <c r="G20" s="1"/>
-      <c r="H20" s="1"/>
-      <c r="I20" s="1"/>
-      <c r="J20" s="1"/>
-      <c r="K20" s="1"/>
+      <c r="D14" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="3">
+        <v>9</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="G14" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>90</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>